<commit_message>
kernel timing for bulk insert
int32 and float64
</commit_message>
<xml_diff>
--- a/test/Performance Data/MGPU/Benchmark_Excel/gtx560Ti/Bulk Insert/gtx560Ti_benchmarkBulkInsert_aleacubase_vs_moderngpu_Float64.xlsx
+++ b/test/Performance Data/MGPU/Benchmark_Excel/gtx560Ti/Bulk Insert/gtx560Ti_benchmarkBulkInsert_aleacubase_vs_moderngpu_Float64.xlsx
@@ -68,10 +68,10 @@
     <t>kernelBulkInsert</t>
   </si>
   <si>
-    <t>Difference</t>
+    <t>kernelMergePartition</t>
   </si>
   <si>
-    <t>kernelMergePartition</t>
+    <t>% Difference</t>
   </si>
 </sst>
 </file>
@@ -544,11 +544,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430660848"/>
-        <c:axId val="1430661936"/>
+        <c:axId val="822498688"/>
+        <c:axId val="822495424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430660848"/>
+        <c:axId val="822498688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -602,12 +602,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430661936"/>
+        <c:crossAx val="822495424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430661936"/>
+        <c:axId val="822495424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430660848"/>
+        <c:crossAx val="822498688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1170,11 +1170,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430659760"/>
-        <c:axId val="1432952896"/>
+        <c:axId val="822491616"/>
+        <c:axId val="822496512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430659760"/>
+        <c:axId val="822491616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,12 +1228,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1432952896"/>
+        <c:crossAx val="822496512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1432952896"/>
+        <c:axId val="822496512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,7 +1287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430659760"/>
+        <c:crossAx val="822491616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1378,6 +1378,2298 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>kernelBulkInsert Timing</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MGPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$32:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.9180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.405000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.430999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>190.71600000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>376.92500000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>935.44799999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1866.144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3727.777</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alea.cuBase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$32:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$32:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.0789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.821</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.289000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.472999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>186.80500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>368.15800000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>911.65200000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1818.883</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3630.4929999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="954861248"/>
+        <c:axId val="950622688"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$31</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Elements</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="34925" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="103000"/>
+                            <a:lumMod val="102000"/>
+                            <a:tint val="94000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent1">
+                            <a:satMod val="110000"/>
+                            <a:lumMod val="100000"/>
+                            <a:shade val="100000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="99000"/>
+                            <a:satMod val="120000"/>
+                            <a:shade val="78000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                        <a:srgbClr val="000000">
+                          <a:alpha val="63000"/>
+                        </a:srgbClr>
+                      </a:outerShdw>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$32:$A$41</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>50000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>200000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>500000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1000000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2000000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5000000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10000000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>20000000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$32:$A$41</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>50000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>200000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>500000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1000000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2000000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5000000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10000000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>20000000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% Difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$32:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$32:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>21.114849504410284</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.622591438790817</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8692169650282326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10132201100067932</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5054709123360648</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0719377200208737</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.353294867820094</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5765795030047034</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5650286958548723</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6442084892236926</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1014069808"/>
+        <c:axId val="1014073616"/>
+      </c:lineChart>
+      <c:valAx>
+        <c:axId val="950622688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="954861248"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="954861248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="950622688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1014073616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Difference</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1014069808"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1014069808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1014073616"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>kernelMergePartition</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Timing</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1024535152"/>
+        <c:axId val="1024537872"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$44</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Elements</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:gradFill rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent1">
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="50000">
+                        <a:schemeClr val="accent1">
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="0"/>
+                  </a:gradFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$45:$A$54</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>10000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>50000</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100000</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>200000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>500000</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1000000</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2000000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5000000</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10000000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>20000000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% Difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$45:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$45:$D$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>46.991783726477614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.49613784907902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.482438016528924</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.566933718852283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.969392416628615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.49905352390882</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.864798563147062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76.439915184560121</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76.724107468874763</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.192440869696171</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1024535152"/>
+        <c:axId val="1024537872"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alea.cuBase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$45:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$45:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.3190000000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.792999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.883000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.295000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.433000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>255.53</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>528.60599999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1108.934</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MGPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$45:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$45:$C$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.7729999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.592000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.670999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.983000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.841999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.606999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.533000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>114.214</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>235.48500000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>491.303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="822583840"/>
+        <c:axId val="822582208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1024535152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Elements</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1024537872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1024537872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Difference</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1024535152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="822582208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="822583840"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="822583840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="822582208"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
   <a:schemeClr val="accent2"/>
@@ -1387,6 +3679,86 @@
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="18">
   <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -2381,6 +4753,1032 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2451,6 +5849,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>80961</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>90486</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2720,12 +6178,264 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:B54"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="V60" sqref="V60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3092,7 +6802,7 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3103,10 +6813,11 @@
         <v>6.0789999999999997</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>4.9180000000000001</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <f>(ABS(B32-C32)/((B32+C32)/2))*100</f>
+        <v>21.114849504410284</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3117,10 +6828,11 @@
         <v>13.821</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>12.18</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <f t="shared" ref="D33:D41" si="0">(ABS(B33-C33)/((B33+C33)/2))*100</f>
+        <v>12.622591438790817</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,10 +6843,11 @@
         <v>23.289000000000001</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>22.405000000000001</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.8692169650282326</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3145,10 +6858,11 @@
         <v>41.472999999999999</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>41.430999999999997</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.10132201100067932</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3159,10 +6873,11 @@
         <v>95.92</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>97.375</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.5054709123360648</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3173,10 +6888,11 @@
         <v>186.80500000000001</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>190.71600000000001</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.0719377200208737</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3187,10 +6903,11 @@
         <v>368.15800000000002</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>376.92500000000001</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.353294867820094</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3201,10 +6918,11 @@
         <v>911.65200000000004</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>935.44799999999998</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5765795030047034</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3215,10 +6933,11 @@
         <v>1818.883</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1866.144</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5650286958548723</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3229,15 +6948,16 @@
         <v>3630.4929999999999</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>3727.777</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.6442084892236926</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3251,7 +6971,7 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3262,10 +6982,11 @@
         <v>9.3190000000000008</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>5.7729999999999997</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <f>(ABS(B45-C45)/((B45+C45)/2))*100</f>
+        <v>46.991783726477614</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3276,10 +6997,11 @@
         <v>25.8</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>14.592000000000001</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <f t="shared" ref="D46:D54" si="1">(ABS(B46-C46)/((B46+C46)/2))*100</f>
+        <v>55.49613784907902</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3290,10 +7012,11 @@
         <v>29.792999999999999</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>16.670999999999999</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>56.482438016528924</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3304,10 +7027,11 @@
         <v>31.82</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>17.983000000000001</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>55.566933718852283</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3318,10 +7042,11 @@
         <v>34.883000000000003</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>19.841999999999999</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>54.969392416628615</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3332,10 +7057,11 @@
         <v>47.295000000000002</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>25.606999999999999</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>59.49905352390882</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3346,10 +7072,11 @@
         <v>93.433000000000007</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>43.533000000000001</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>72.864798563147062</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3360,10 +7087,11 @@
         <v>255.53</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>114.214</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>76.439915184560121</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3374,10 +7102,11 @@
         <v>528.60599999999999</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>235.48500000000001</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>76.724107468874763</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3388,10 +7117,11 @@
         <v>1108.934</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>491.303</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>77.192440869696171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>